<commit_message>
Put spaces in example names
</commit_message>
<xml_diff>
--- a/docs/tests/metadata_multiplexed.xlsx
+++ b/docs/tests/metadata_multiplexed.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/Dropbox (Personal)/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/GitHub/steinbaugh/basejump/docs/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -71,31 +71,31 @@
     <t>run2_R1.fastq.gz</t>
   </si>
   <si>
-    <t>run1</t>
-  </si>
-  <si>
-    <t>run2</t>
-  </si>
-  <si>
-    <t>sample1</t>
-  </si>
-  <si>
-    <t>sample2</t>
-  </si>
-  <si>
-    <t>sample3</t>
-  </si>
-  <si>
-    <t>sample4</t>
-  </si>
-  <si>
-    <t>sample5</t>
-  </si>
-  <si>
-    <t>sample6</t>
-  </si>
-  <si>
-    <t>sample7</t>
+    <t>run 1</t>
+  </si>
+  <si>
+    <t>run 2</t>
+  </si>
+  <si>
+    <t>sample 1</t>
+  </si>
+  <si>
+    <t>sample 2</t>
+  </si>
+  <si>
+    <t>sample 3</t>
+  </si>
+  <si>
+    <t>sample 4</t>
+  </si>
+  <si>
+    <t>sample 5</t>
+  </si>
+  <si>
+    <t>sample 6</t>
+  </si>
+  <si>
+    <t>sample 7</t>
   </si>
 </sst>
 </file>
@@ -447,16 +447,16 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" style="2"/>
-    <col min="5" max="5" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="10.7109375" style="2"/>
   </cols>
   <sheetData>

</xml_diff>